<commit_message>
Updates to Canada inventory scaling 1. added mapping file for NOx. NOx agriculture emissions from CEDS are no longer scaled to CAN inventory AGR sectors for soil and manure management (zero in inventory). This corrects a previous underprediction in CAN AGR NOx. 2. Added mapping file for CO so that CO waste emissions are better captured in the scaling process.
</commit_message>
<xml_diff>
--- a/input/mappings/scaling/CAN_scaling_mapping_2017Update.xlsx
+++ b/input/mappings/scaling/CAN_scaling_mapping_2017Update.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10715"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11110"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/emcduffie/Documents/GEOS-Chem/CEDS_Emissions/CEDS_v0611/input/mappings/scaling/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/emcduffie/Documents/GEOS-Chem/CEDS/CEDS_v0611/input/mappings/scaling/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50A1196F-90E8-1841-B8BD-F758ECC43F09}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A45E3CBF-D6E2-E94F-8B9C-6CB4398C8A06}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13400" yWindow="8040" windowWidth="25000" windowHeight="14420" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="map" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="327" uniqueCount="253">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="330" uniqueCount="254">
   <si>
     <t>inv_sector</t>
   </si>
@@ -786,6 +786,9 @@
   </si>
   <si>
     <t xml:space="preserve">Metal Mining </t>
+  </si>
+  <si>
+    <t>NOTE: CEDS 6A emissions are zero, so scaling sector 6A = 0 emissions too</t>
   </si>
 </sst>
 </file>
@@ -2054,7 +2057,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D208"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A91" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A80" workbookViewId="0">
       <selection activeCell="B107" sqref="B107"/>
     </sheetView>
   </sheetViews>
@@ -2961,12 +2964,9 @@
       <c r="A128" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="B128" t="s">
-        <v>26</v>
-      </c>
       <c r="C128" s="1"/>
     </row>
-    <row r="129" spans="1:3">
+    <row r="129" spans="1:4">
       <c r="B129" t="s">
         <v>26</v>
       </c>
@@ -2974,7 +2974,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="130" spans="1:3">
+    <row r="130" spans="1:4">
       <c r="B130" t="s">
         <v>26</v>
       </c>
@@ -2982,7 +2982,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="131" spans="1:3">
+    <row r="131" spans="1:4">
       <c r="B131" t="s">
         <v>26</v>
       </c>
@@ -2990,7 +2990,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="132" spans="1:3">
+    <row r="132" spans="1:4">
       <c r="B132" t="s">
         <v>26</v>
       </c>
@@ -2998,7 +2998,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="133" spans="1:3">
+    <row r="133" spans="1:4">
       <c r="B133" t="s">
         <v>26</v>
       </c>
@@ -3006,47 +3006,56 @@
         <v>64</v>
       </c>
     </row>
-    <row r="134" spans="1:3">
+    <row r="134" spans="1:4">
       <c r="A134" s="10" t="s">
         <v>229</v>
       </c>
-    </row>
-    <row r="135" spans="1:3">
+      <c r="B134" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="135" spans="1:4">
       <c r="A135" s="11" t="s">
         <v>230</v>
       </c>
-    </row>
-    <row r="136" spans="1:3">
+      <c r="B135" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="136" spans="1:4">
       <c r="A136" s="12" t="s">
         <v>231</v>
       </c>
     </row>
-    <row r="137" spans="1:3">
+    <row r="137" spans="1:4">
       <c r="A137" s="12" t="s">
         <v>232</v>
       </c>
     </row>
-    <row r="138" spans="1:3">
+    <row r="138" spans="1:4">
       <c r="A138" s="12" t="s">
         <v>233</v>
       </c>
     </row>
-    <row r="139" spans="1:3">
+    <row r="139" spans="1:4">
       <c r="A139" s="12" t="s">
         <v>234</v>
       </c>
     </row>
-    <row r="140" spans="1:3">
+    <row r="140" spans="1:4">
       <c r="A140" s="13" t="s">
         <v>235</v>
       </c>
-    </row>
-    <row r="143" spans="1:3">
+      <c r="B140" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="143" spans="1:4">
       <c r="A143" s="2" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="144" spans="1:3">
+    <row r="144" spans="1:4">
       <c r="A144" s="10" t="s">
         <v>19</v>
       </c>
@@ -3055,6 +3064,9 @@
       </c>
       <c r="C144" s="1" t="s">
         <v>57</v>
+      </c>
+      <c r="D144" t="s">
+        <v>253</v>
       </c>
     </row>
     <row r="145" spans="1:3">
@@ -3124,7 +3136,7 @@
         <v>144</v>
       </c>
       <c r="B152" t="s">
-        <v>103</v>
+        <v>51</v>
       </c>
       <c r="C152" s="4"/>
     </row>

</xml_diff>